<commit_message>
Update Proyectos por Coordinados.xlsx
</commit_message>
<xml_diff>
--- a/Personal/Proyectos por Coordinados.xlsx
+++ b/Personal/Proyectos por Coordinados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepositorioORFEI\Gestion-ORFEI\Personal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F542D90-91E4-4FFF-9749-9DCFEA7985CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112373F0-042B-4EEB-8FB9-9A3FBA411282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="852" windowWidth="30000" windowHeight="16428" tabRatio="504" xr2:uid="{52105EA4-0312-4C00-B0B6-7ED9E8BCD461}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="504" xr2:uid="{52105EA4-0312-4C00-B0B6-7ED9E8BCD461}"/>
   </bookViews>
   <sheets>
     <sheet name="Peogramacion " sheetId="2" r:id="rId1"/>
@@ -200,9 +200,6 @@
     <t>Obstetra</t>
   </si>
   <si>
-    <t>Jhon Palomino</t>
-  </si>
-  <si>
     <t>Formulador</t>
   </si>
   <si>
@@ -216,6 +213,9 @@
   </si>
   <si>
     <t>MEJORAMIENTO DEL SERVICIO EDUCATIVO DEL NIVEL INICIAL N°1135 SANGABRIEL, N°171 PICHIUPATA, N° 39 HUANCARAMA, N° 938 HUACCAYHURA, DISTRITO DE HUANCARAMA PROVINCIA DE ANDAHUAYLAS, REGION APURIMAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                </t>
   </si>
 </sst>
 </file>
@@ -762,7 +762,7 @@
   <dimension ref="A1:J84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,7 +834,7 @@
         <v>41</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>44</v>
@@ -846,10 +846,10 @@
         <v>43</v>
       </c>
       <c r="G3" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>55</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>56</v>
       </c>
       <c r="I3" s="15">
         <v>44022</v>
@@ -868,10 +868,10 @@
         <v>46</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I4" s="15">
         <v>44063</v>
@@ -890,10 +890,10 @@
         <v>48</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I5" s="15">
         <v>44114</v>
@@ -930,7 +930,7 @@
       <c r="A8" s="29"/>
       <c r="B8" s="29"/>
       <c r="C8" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>44</v>

</xml_diff>